<commit_message>
add: aula 4 inteligencia artificial
</commit_message>
<xml_diff>
--- a/Aula 3/Produtos.xlsx
+++ b/Aula 3/Produtos.xlsx
@@ -462,16 +462,16 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>5.18</v>
+        <v>5.2</v>
       </c>
       <c r="E2">
-        <v>5179.9482</v>
+        <v>5199.948</v>
       </c>
       <c r="F2">
         <v>1.4</v>
       </c>
       <c r="G2">
-        <v>7251.927479999999</v>
+        <v>7279.9272</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,16 +485,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>5.61</v>
+        <v>5.65</v>
       </c>
       <c r="E3">
-        <v>25245</v>
+        <v>25425</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>50490</v>
+        <v>50850</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -508,16 +508,16 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5.18</v>
+        <v>5.2</v>
       </c>
       <c r="E4">
-        <v>4661.9482</v>
+        <v>4679.948</v>
       </c>
       <c r="F4">
         <v>1.7</v>
       </c>
       <c r="G4">
-        <v>7925.31194</v>
+        <v>7955.9116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -531,16 +531,16 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>5.18</v>
+        <v>5.2</v>
       </c>
       <c r="E5">
-        <v>4138.82</v>
+        <v>4154.8</v>
       </c>
       <c r="F5">
         <v>1.7</v>
       </c>
       <c r="G5">
-        <v>7035.994</v>
+        <v>7063.16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -554,16 +554,16 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>5.61</v>
+        <v>5.65</v>
       </c>
       <c r="E6">
-        <v>16830</v>
+        <v>16950</v>
       </c>
       <c r="F6">
         <v>1.9</v>
       </c>
       <c r="G6">
-        <v>31977</v>
+        <v>32205</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -577,16 +577,16 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>5.18</v>
+        <v>5.2</v>
       </c>
       <c r="E7">
-        <v>2488.8864</v>
+        <v>2498.496</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>4977.7728</v>
+        <v>4996.992</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -600,16 +600,16 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>321.72</v>
+        <v>321.82</v>
       </c>
       <c r="E8">
-        <v>6434.400000000001</v>
+        <v>6436.4</v>
       </c>
       <c r="F8">
         <v>1.15</v>
       </c>
       <c r="G8">
-        <v>7399.56</v>
+        <v>7401.859999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>